<commit_message>
main_menu change, youtube ui ver0.1, youtube fullscreen possible, community ui change
</commit_message>
<xml_diff>
--- a/스케줄.xlsx
+++ b/스케줄.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Red\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Red\Desktop\Yofficial\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -847,27 +847,114 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="24" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="9" fontId="24" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -879,125 +966,38 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="24" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="24" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1286,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC33" sqref="AC33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1307,99 +1307,99 @@
       <c r="F19" s="19"/>
     </row>
     <row r="20" spans="4:29">
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="43"/>
-      <c r="T20" s="43"/>
-      <c r="U20" s="43"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="43"/>
-      <c r="X20" s="43"/>
-      <c r="Y20" s="43"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="52"/>
+      <c r="P20" s="52"/>
+      <c r="Q20" s="52"/>
+      <c r="R20" s="52"/>
+      <c r="S20" s="52"/>
+      <c r="T20" s="52"/>
+      <c r="U20" s="52"/>
+      <c r="V20" s="52"/>
+      <c r="W20" s="52"/>
+      <c r="X20" s="52"/>
+      <c r="Y20" s="52"/>
     </row>
     <row r="21" spans="4:29">
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="45"/>
-      <c r="U21" s="45"/>
-      <c r="V21" s="45"/>
-      <c r="W21" s="45"/>
-      <c r="X21" s="45"/>
-      <c r="Y21" s="45"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="54"/>
+      <c r="U21" s="54"/>
+      <c r="V21" s="54"/>
+      <c r="W21" s="54"/>
+      <c r="X21" s="54"/>
+      <c r="Y21" s="54"/>
     </row>
     <row r="22" spans="4:29">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="50" t="s">
+      <c r="F22" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="51" t="s">
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="J22" s="52"/>
-      <c r="K22" s="55" t="s">
+      <c r="J22" s="61"/>
+      <c r="K22" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="46" t="s">
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="P22" s="47"/>
-      <c r="Q22" s="47"/>
-      <c r="R22" s="47"/>
-      <c r="S22" s="56"/>
-      <c r="T22" s="59" t="s">
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="65"/>
+      <c r="T22" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="U22" s="47"/>
-      <c r="V22" s="47"/>
-      <c r="W22" s="47"/>
-      <c r="X22" s="46" t="s">
+      <c r="U22" s="45"/>
+      <c r="V22" s="45"/>
+      <c r="W22" s="45"/>
+      <c r="X22" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="Y22" s="47"/>
+      <c r="Y22" s="45"/>
     </row>
     <row r="23" spans="4:29">
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="54"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="63"/>
       <c r="K23" s="4">
         <v>4</v>
       </c>
@@ -1448,758 +1448,758 @@
     </row>
     <row r="24" spans="4:29" ht="17.25" customHeight="1">
       <c r="D24" s="20"/>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="62" t="s">
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="J24" s="62"/>
-      <c r="K24" s="33" t="s">
+      <c r="J24" s="81"/>
+      <c r="K24" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
       <c r="O24" s="17"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
-      <c r="R24" s="60" t="s">
+      <c r="R24" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="S24" s="28" t="s">
+      <c r="S24" s="74" t="s">
         <v>11</v>
       </c>
       <c r="T24" s="8"/>
       <c r="U24" s="8"/>
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
-      <c r="X24" s="28" t="s">
+      <c r="X24" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="Y24" s="30" t="s">
+      <c r="Y24" s="76" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="4:29" ht="30" customHeight="1">
       <c r="D25" s="20"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="63" t="s">
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="63"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="80"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="80"/>
       <c r="O25" s="8"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="8"/>
-      <c r="R25" s="61"/>
-      <c r="S25" s="29"/>
+      <c r="R25" s="48"/>
+      <c r="S25" s="75"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
-      <c r="X25" s="29"/>
-      <c r="Y25" s="31"/>
+      <c r="X25" s="75"/>
+      <c r="Y25" s="77"/>
     </row>
     <row r="26" spans="4:29" ht="30" customHeight="1">
       <c r="D26" s="20"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="63" t="s">
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="63"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="80"/>
+      <c r="L26" s="80"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="80"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
-      <c r="R26" s="61"/>
-      <c r="S26" s="29"/>
-      <c r="T26" s="66"/>
+      <c r="R26" s="48"/>
+      <c r="S26" s="75"/>
+      <c r="T26" s="30"/>
       <c r="U26" s="8"/>
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
-      <c r="X26" s="29"/>
-      <c r="Y26" s="31"/>
-      <c r="AA26" s="74"/>
-      <c r="AB26" s="74"/>
-      <c r="AC26" s="74"/>
+      <c r="X26" s="75"/>
+      <c r="Y26" s="77"/>
+      <c r="AA26" s="35"/>
+      <c r="AB26" s="35"/>
+      <c r="AC26" s="35"/>
     </row>
     <row r="27" spans="4:29" ht="17.45" customHeight="1">
       <c r="D27" s="20"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="63" t="s">
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="J27" s="63"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="80"/>
+      <c r="L27" s="80"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="80"/>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="17"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="29"/>
+      <c r="R27" s="48"/>
+      <c r="S27" s="75"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
-      <c r="X27" s="29"/>
-      <c r="Y27" s="31"/>
-      <c r="AA27" s="74"/>
-      <c r="AB27" s="74"/>
-      <c r="AC27" s="74"/>
+      <c r="X27" s="75"/>
+      <c r="Y27" s="77"/>
+      <c r="AA27" s="35"/>
+      <c r="AB27" s="35"/>
+      <c r="AC27" s="35"/>
     </row>
     <row r="28" spans="4:29" ht="17.45" customHeight="1">
       <c r="D28" s="20"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="63" t="s">
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="J28" s="63"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="80"/>
+      <c r="M28" s="80"/>
+      <c r="N28" s="80"/>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="17"/>
-      <c r="R28" s="61"/>
-      <c r="S28" s="29"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="75"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
       <c r="V28" s="8"/>
       <c r="W28" s="8"/>
-      <c r="X28" s="29"/>
-      <c r="Y28" s="31"/>
-      <c r="AA28" s="74"/>
-      <c r="AB28" s="74"/>
-      <c r="AC28" s="74"/>
+      <c r="X28" s="75"/>
+      <c r="Y28" s="77"/>
+      <c r="AA28" s="35"/>
+      <c r="AB28" s="35"/>
+      <c r="AC28" s="35"/>
     </row>
     <row r="29" spans="4:29" ht="17.45" customHeight="1">
       <c r="D29" s="20"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="63" t="s">
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="J29" s="63"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="34"/>
-      <c r="N29" s="34"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="80"/>
+      <c r="M29" s="80"/>
+      <c r="N29" s="80"/>
       <c r="O29" s="8"/>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
-      <c r="R29" s="61"/>
-      <c r="S29" s="29"/>
-      <c r="T29" s="65"/>
+      <c r="R29" s="48"/>
+      <c r="S29" s="75"/>
+      <c r="T29" s="29"/>
       <c r="U29" s="8"/>
       <c r="V29" s="8"/>
       <c r="W29" s="8"/>
-      <c r="X29" s="29"/>
-      <c r="Y29" s="31"/>
-      <c r="AA29" s="75"/>
-      <c r="AB29" s="75"/>
-      <c r="AC29" s="74"/>
+      <c r="X29" s="75"/>
+      <c r="Y29" s="77"/>
+      <c r="AA29" s="38"/>
+      <c r="AB29" s="38"/>
+      <c r="AC29" s="35"/>
     </row>
     <row r="30" spans="4:29" ht="17.45" customHeight="1">
       <c r="D30" s="10"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="63" t="s">
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="J30" s="63"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="80"/>
+      <c r="L30" s="80"/>
+      <c r="M30" s="80"/>
+      <c r="N30" s="80"/>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
-      <c r="R30" s="61"/>
-      <c r="S30" s="29"/>
-      <c r="T30" s="66"/>
-      <c r="U30" s="66"/>
+      <c r="R30" s="48"/>
+      <c r="S30" s="75"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="30"/>
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
-      <c r="X30" s="29"/>
-      <c r="Y30" s="31"/>
-      <c r="AA30" s="74"/>
-      <c r="AB30" s="74"/>
-      <c r="AC30" s="74"/>
+      <c r="X30" s="75"/>
+      <c r="Y30" s="77"/>
+      <c r="AA30" s="35"/>
+      <c r="AB30" s="35"/>
+      <c r="AC30" s="35"/>
     </row>
     <row r="31" spans="4:29" ht="17.45" customHeight="1">
       <c r="D31" s="10"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="63" t="s">
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="70"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="80"/>
+      <c r="M31" s="80"/>
+      <c r="N31" s="80"/>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
       <c r="Q31" s="8"/>
-      <c r="R31" s="61"/>
-      <c r="S31" s="29"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="75"/>
       <c r="T31" s="8"/>
       <c r="U31" s="8"/>
-      <c r="V31" s="66"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="29"/>
-      <c r="Y31" s="31"/>
-      <c r="AA31" s="74"/>
-      <c r="AB31" s="74"/>
-      <c r="AC31" s="74"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="30"/>
+      <c r="X31" s="75"/>
+      <c r="Y31" s="77"/>
+      <c r="AA31" s="35"/>
+      <c r="AB31" s="35"/>
+      <c r="AC31" s="35"/>
     </row>
     <row r="32" spans="4:29" ht="17.45" customHeight="1">
       <c r="D32" s="10"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="63" t="s">
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="J32" s="70"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
+      <c r="M32" s="80"/>
+      <c r="N32" s="80"/>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
       <c r="Q32" s="8"/>
-      <c r="R32" s="61"/>
-      <c r="S32" s="29"/>
+      <c r="R32" s="48"/>
+      <c r="S32" s="75"/>
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
-      <c r="V32" s="65"/>
+      <c r="V32" s="29"/>
       <c r="W32" s="8"/>
-      <c r="X32" s="29"/>
-      <c r="Y32" s="31"/>
-      <c r="AA32" s="74"/>
-      <c r="AB32" s="74"/>
-      <c r="AC32" s="74"/>
+      <c r="X32" s="75"/>
+      <c r="Y32" s="77"/>
+      <c r="AA32" s="35"/>
+      <c r="AB32" s="35"/>
+      <c r="AC32" s="8"/>
     </row>
     <row r="33" spans="4:26" ht="17.45" customHeight="1" thickBot="1">
       <c r="D33" s="10"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="71" t="s">
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="J33" s="71"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="80"/>
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
       <c r="Q33" s="8"/>
-      <c r="R33" s="61"/>
-      <c r="S33" s="29"/>
+      <c r="R33" s="48"/>
+      <c r="S33" s="75"/>
       <c r="T33" s="8"/>
       <c r="U33" s="8"/>
       <c r="V33" s="8"/>
-      <c r="W33" s="66"/>
-      <c r="X33" s="29"/>
-      <c r="Y33" s="31"/>
+      <c r="W33" s="30"/>
+      <c r="X33" s="75"/>
+      <c r="Y33" s="77"/>
     </row>
     <row r="34" spans="4:26" ht="24.75" customHeight="1">
-      <c r="D34" s="57"/>
-      <c r="E34" s="77" t="s">
+      <c r="D34" s="41"/>
+      <c r="E34" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="40" t="s">
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="40"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="80"/>
+      <c r="N34" s="80"/>
       <c r="O34" s="16"/>
       <c r="P34" s="21"/>
       <c r="Q34" s="21"/>
-      <c r="R34" s="61"/>
-      <c r="S34" s="29"/>
+      <c r="R34" s="48"/>
+      <c r="S34" s="75"/>
       <c r="T34" s="9"/>
       <c r="U34" s="9"/>
       <c r="V34" s="9"/>
       <c r="W34" s="9"/>
-      <c r="X34" s="29"/>
-      <c r="Y34" s="31"/>
+      <c r="X34" s="75"/>
+      <c r="Y34" s="77"/>
       <c r="Z34" s="12"/>
     </row>
     <row r="35" spans="4:26">
-      <c r="D35" s="72"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="40" t="s">
+      <c r="D35" s="42"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="J35" s="40"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="34"/>
-      <c r="N35" s="34"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
+      <c r="N35" s="80"/>
       <c r="O35" s="21"/>
       <c r="P35" s="16"/>
       <c r="Q35" s="21"/>
-      <c r="R35" s="61"/>
-      <c r="S35" s="29"/>
-      <c r="T35" s="64"/>
+      <c r="R35" s="48"/>
+      <c r="S35" s="75"/>
+      <c r="T35" s="28"/>
       <c r="U35" s="9"/>
       <c r="V35" s="9"/>
       <c r="W35" s="9"/>
-      <c r="X35" s="29"/>
-      <c r="Y35" s="31"/>
+      <c r="X35" s="75"/>
+      <c r="Y35" s="77"/>
       <c r="Z35" s="12"/>
     </row>
     <row r="36" spans="4:26" ht="17.45" customHeight="1">
-      <c r="D36" s="72"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
-      <c r="I36" s="40" t="s">
+      <c r="D36" s="42"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="J36" s="40"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="80"/>
+      <c r="M36" s="80"/>
+      <c r="N36" s="80"/>
       <c r="O36" s="21"/>
       <c r="P36" s="21"/>
       <c r="Q36" s="16"/>
-      <c r="R36" s="61"/>
-      <c r="S36" s="29"/>
+      <c r="R36" s="48"/>
+      <c r="S36" s="75"/>
       <c r="T36" s="9"/>
       <c r="U36" s="9"/>
       <c r="V36" s="9"/>
       <c r="W36" s="9"/>
-      <c r="X36" s="29"/>
-      <c r="Y36" s="31"/>
+      <c r="X36" s="75"/>
+      <c r="Y36" s="77"/>
       <c r="Z36" s="12"/>
     </row>
     <row r="37" spans="4:26" ht="29.25" customHeight="1">
-      <c r="D37" s="58"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="40" t="s">
+      <c r="D37" s="43"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="J37" s="40"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="64"/>
-      <c r="P37" s="64"/>
-      <c r="Q37" s="64"/>
-      <c r="R37" s="61"/>
-      <c r="S37" s="29"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="80"/>
+      <c r="L37" s="80"/>
+      <c r="M37" s="80"/>
+      <c r="N37" s="80"/>
+      <c r="O37" s="28"/>
+      <c r="P37" s="28"/>
+      <c r="Q37" s="28"/>
+      <c r="R37" s="48"/>
+      <c r="S37" s="75"/>
       <c r="T37" s="14"/>
-      <c r="U37" s="73"/>
-      <c r="V37" s="64"/>
-      <c r="W37" s="64"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="31"/>
+      <c r="U37" s="34"/>
+      <c r="V37" s="28"/>
+      <c r="W37" s="28"/>
+      <c r="X37" s="75"/>
+      <c r="Y37" s="77"/>
       <c r="Z37" s="12"/>
     </row>
     <row r="38" spans="4:26">
       <c r="D38" s="23"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="78"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="40" t="s">
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="J38" s="40"/>
-      <c r="K38" s="34"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="64"/>
-      <c r="P38" s="64"/>
-      <c r="Q38" s="64"/>
-      <c r="R38" s="61"/>
-      <c r="S38" s="29"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="80"/>
+      <c r="L38" s="80"/>
+      <c r="M38" s="80"/>
+      <c r="N38" s="80"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="28"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="48"/>
+      <c r="S38" s="75"/>
       <c r="T38" s="14"/>
-      <c r="U38" s="73"/>
-      <c r="V38" s="64"/>
-      <c r="W38" s="64"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="31"/>
+      <c r="U38" s="34"/>
+      <c r="V38" s="28"/>
+      <c r="W38" s="28"/>
+      <c r="X38" s="75"/>
+      <c r="Y38" s="77"/>
       <c r="Z38" s="12"/>
     </row>
     <row r="39" spans="4:26" ht="29.25" customHeight="1">
       <c r="D39" s="23"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="40" t="s">
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="J39" s="40"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="64"/>
-      <c r="P39" s="64"/>
-      <c r="Q39" s="64"/>
-      <c r="R39" s="61"/>
-      <c r="S39" s="29"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="80"/>
+      <c r="L39" s="80"/>
+      <c r="M39" s="80"/>
+      <c r="N39" s="80"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="48"/>
+      <c r="S39" s="75"/>
       <c r="T39" s="14"/>
-      <c r="U39" s="73"/>
-      <c r="V39" s="64"/>
-      <c r="W39" s="64"/>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="31"/>
+      <c r="U39" s="34"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="28"/>
+      <c r="X39" s="75"/>
+      <c r="Y39" s="77"/>
       <c r="Z39" s="12"/>
     </row>
     <row r="40" spans="4:26" ht="29.25" customHeight="1">
       <c r="D40" s="23"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="40" t="s">
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="J40" s="40"/>
-      <c r="K40" s="34"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
-      <c r="O40" s="64"/>
-      <c r="P40" s="64"/>
-      <c r="Q40" s="64"/>
-      <c r="R40" s="61"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="64"/>
-      <c r="U40" s="22"/>
-      <c r="V40" s="64"/>
-      <c r="W40" s="64"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="31"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="80"/>
+      <c r="L40" s="80"/>
+      <c r="M40" s="80"/>
+      <c r="N40" s="80"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="48"/>
+      <c r="S40" s="75"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="22"/>
+      <c r="W40" s="22"/>
+      <c r="X40" s="75"/>
+      <c r="Y40" s="77"/>
       <c r="Z40" s="12"/>
     </row>
     <row r="41" spans="4:26" ht="29.25" customHeight="1">
       <c r="D41" s="23"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="40" t="s">
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="J41" s="40"/>
-      <c r="K41" s="34"/>
-      <c r="L41" s="34"/>
-      <c r="M41" s="34"/>
-      <c r="N41" s="34"/>
-      <c r="O41" s="64"/>
-      <c r="P41" s="64"/>
-      <c r="Q41" s="64"/>
-      <c r="R41" s="61"/>
-      <c r="S41" s="29"/>
-      <c r="T41" s="64"/>
-      <c r="U41" s="22"/>
-      <c r="V41" s="64"/>
-      <c r="W41" s="64"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="31"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="80"/>
+      <c r="L41" s="80"/>
+      <c r="M41" s="80"/>
+      <c r="N41" s="80"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="28"/>
+      <c r="R41" s="48"/>
+      <c r="S41" s="75"/>
+      <c r="T41" s="28"/>
+      <c r="U41" s="28"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="28"/>
+      <c r="X41" s="75"/>
+      <c r="Y41" s="77"/>
       <c r="Z41" s="12"/>
     </row>
     <row r="42" spans="4:26" ht="29.25" customHeight="1">
       <c r="D42" s="23"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="40" t="s">
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="J42" s="40"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="34"/>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
-      <c r="O42" s="64"/>
-      <c r="P42" s="64"/>
-      <c r="Q42" s="64"/>
-      <c r="R42" s="61"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="64"/>
-      <c r="U42" s="73"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="31"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="80"/>
+      <c r="L42" s="80"/>
+      <c r="M42" s="80"/>
+      <c r="N42" s="80"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="48"/>
+      <c r="S42" s="75"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="28"/>
+      <c r="X42" s="75"/>
+      <c r="Y42" s="77"/>
       <c r="Z42" s="12"/>
     </row>
     <row r="43" spans="4:26" ht="29.25" customHeight="1" thickBot="1">
       <c r="D43" s="23"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="40" t="s">
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="J43" s="40"/>
-      <c r="K43" s="34"/>
-      <c r="L43" s="34"/>
-      <c r="M43" s="34"/>
-      <c r="N43" s="34"/>
-      <c r="O43" s="64"/>
-      <c r="P43" s="64"/>
-      <c r="Q43" s="64"/>
-      <c r="R43" s="61"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="64"/>
-      <c r="U43" s="73"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="80"/>
+      <c r="L43" s="80"/>
+      <c r="M43" s="80"/>
+      <c r="N43" s="80"/>
+      <c r="O43" s="28"/>
+      <c r="P43" s="28"/>
+      <c r="Q43" s="28"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="75"/>
+      <c r="T43" s="28"/>
+      <c r="U43" s="34"/>
       <c r="V43" s="14"/>
       <c r="W43" s="14"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="31"/>
+      <c r="X43" s="75"/>
+      <c r="Y43" s="77"/>
       <c r="Z43" s="12"/>
     </row>
     <row r="44" spans="4:26" ht="18.75" customHeight="1">
-      <c r="D44" s="35"/>
-      <c r="E44" s="79" t="s">
+      <c r="D44" s="66"/>
+      <c r="E44" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="79"/>
-      <c r="G44" s="79"/>
-      <c r="H44" s="79"/>
-      <c r="I44" s="37" t="s">
+      <c r="F44" s="71"/>
+      <c r="G44" s="71"/>
+      <c r="H44" s="71"/>
+      <c r="I44" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="J44" s="37"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="34"/>
-      <c r="M44" s="34"/>
-      <c r="N44" s="34"/>
+      <c r="J44" s="68"/>
+      <c r="K44" s="80"/>
+      <c r="L44" s="80"/>
+      <c r="M44" s="80"/>
+      <c r="N44" s="80"/>
       <c r="O44" s="18"/>
-      <c r="P44" s="64"/>
-      <c r="Q44" s="64"/>
-      <c r="R44" s="61"/>
-      <c r="S44" s="29"/>
+      <c r="P44" s="28"/>
+      <c r="Q44" s="28"/>
+      <c r="R44" s="48"/>
+      <c r="S44" s="75"/>
       <c r="T44" s="9"/>
       <c r="U44" s="9"/>
       <c r="V44" s="9"/>
       <c r="W44" s="9"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="31"/>
+      <c r="X44" s="75"/>
+      <c r="Y44" s="77"/>
       <c r="Z44" s="12"/>
     </row>
     <row r="45" spans="4:26" ht="18.75" customHeight="1">
-      <c r="D45" s="35"/>
-      <c r="E45" s="80"/>
-      <c r="F45" s="80"/>
-      <c r="G45" s="80"/>
-      <c r="H45" s="80"/>
-      <c r="I45" s="41" t="s">
+      <c r="D45" s="66"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="J45" s="47"/>
-      <c r="K45" s="34"/>
-      <c r="L45" s="34"/>
-      <c r="M45" s="34"/>
-      <c r="N45" s="34"/>
-      <c r="O45" s="64"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="80"/>
+      <c r="L45" s="80"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="28"/>
       <c r="P45" s="18"/>
-      <c r="Q45" s="64"/>
-      <c r="R45" s="61"/>
-      <c r="S45" s="29"/>
-      <c r="T45" s="64"/>
+      <c r="Q45" s="28"/>
+      <c r="R45" s="48"/>
+      <c r="S45" s="75"/>
+      <c r="T45" s="28"/>
       <c r="U45" s="9"/>
       <c r="V45" s="9"/>
       <c r="W45" s="9"/>
-      <c r="X45" s="29"/>
-      <c r="Y45" s="31"/>
+      <c r="X45" s="75"/>
+      <c r="Y45" s="77"/>
       <c r="Z45" s="12"/>
     </row>
     <row r="46" spans="4:26" ht="18.75" customHeight="1">
-      <c r="D46" s="35"/>
-      <c r="E46" s="80"/>
-      <c r="F46" s="80"/>
-      <c r="G46" s="80"/>
-      <c r="H46" s="80"/>
-      <c r="I46" s="41" t="s">
+      <c r="D46" s="66"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="72"/>
+      <c r="I46" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="J46" s="41"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
-      <c r="O46" s="64"/>
-      <c r="P46" s="64"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="80"/>
+      <c r="L46" s="80"/>
+      <c r="M46" s="80"/>
+      <c r="N46" s="80"/>
+      <c r="O46" s="28"/>
+      <c r="P46" s="28"/>
       <c r="Q46" s="18"/>
-      <c r="R46" s="61"/>
-      <c r="S46" s="29"/>
+      <c r="R46" s="48"/>
+      <c r="S46" s="75"/>
       <c r="T46" s="18"/>
       <c r="U46" s="9"/>
       <c r="V46" s="9"/>
       <c r="W46" s="9"/>
-      <c r="X46" s="29"/>
-      <c r="Y46" s="31"/>
+      <c r="X46" s="75"/>
+      <c r="Y46" s="77"/>
       <c r="Z46" s="12"/>
     </row>
     <row r="47" spans="4:26" ht="18.75" customHeight="1">
-      <c r="D47" s="35"/>
-      <c r="E47" s="80"/>
-      <c r="F47" s="80"/>
-      <c r="G47" s="80"/>
-      <c r="H47" s="80"/>
-      <c r="I47" s="41" t="s">
+      <c r="D47" s="66"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="72"/>
+      <c r="I47" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="J47" s="47"/>
-      <c r="K47" s="34"/>
-      <c r="L47" s="34"/>
-      <c r="M47" s="34"/>
-      <c r="N47" s="34"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="80"/>
+      <c r="L47" s="80"/>
+      <c r="M47" s="80"/>
+      <c r="N47" s="80"/>
       <c r="O47" s="9"/>
-      <c r="P47" s="64"/>
-      <c r="Q47" s="69"/>
-      <c r="R47" s="61"/>
-      <c r="S47" s="29"/>
+      <c r="P47" s="28"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="48"/>
+      <c r="S47" s="75"/>
       <c r="T47" s="18"/>
-      <c r="U47" s="64"/>
-      <c r="V47" s="64"/>
-      <c r="W47" s="64"/>
-      <c r="X47" s="29"/>
-      <c r="Y47" s="31"/>
+      <c r="U47" s="28"/>
+      <c r="V47" s="28"/>
+      <c r="W47" s="28"/>
+      <c r="X47" s="75"/>
+      <c r="Y47" s="77"/>
       <c r="Z47" s="12"/>
     </row>
     <row r="48" spans="4:26" ht="18.75" customHeight="1">
-      <c r="D48" s="35"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="80"/>
-      <c r="I48" s="41" t="s">
+      <c r="D48" s="66"/>
+      <c r="E48" s="72"/>
+      <c r="F48" s="72"/>
+      <c r="G48" s="72"/>
+      <c r="H48" s="72"/>
+      <c r="I48" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="41"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="34"/>
-      <c r="N48" s="34"/>
+      <c r="J48" s="49"/>
+      <c r="K48" s="80"/>
+      <c r="L48" s="80"/>
+      <c r="M48" s="80"/>
+      <c r="N48" s="80"/>
       <c r="O48" s="24"/>
-      <c r="P48" s="68"/>
-      <c r="Q48" s="69"/>
-      <c r="R48" s="61"/>
-      <c r="S48" s="29"/>
-      <c r="T48" s="68"/>
+      <c r="P48" s="32"/>
+      <c r="Q48" s="33"/>
+      <c r="R48" s="48"/>
+      <c r="S48" s="75"/>
+      <c r="T48" s="32"/>
       <c r="U48" s="25"/>
-      <c r="V48" s="68"/>
-      <c r="W48" s="68"/>
-      <c r="X48" s="29"/>
-      <c r="Y48" s="31"/>
+      <c r="V48" s="32"/>
+      <c r="W48" s="32"/>
+      <c r="X48" s="75"/>
+      <c r="Y48" s="77"/>
       <c r="Z48" s="12"/>
     </row>
     <row r="49" spans="4:26" ht="18.75" customHeight="1">
-      <c r="D49" s="35"/>
-      <c r="E49" s="80"/>
-      <c r="F49" s="80"/>
-      <c r="G49" s="80"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="41" t="s">
+      <c r="D49" s="66"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="72"/>
+      <c r="H49" s="72"/>
+      <c r="I49" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="J49" s="41"/>
-      <c r="K49" s="34"/>
-      <c r="L49" s="34"/>
-      <c r="M49" s="34"/>
-      <c r="N49" s="34"/>
+      <c r="J49" s="49"/>
+      <c r="K49" s="80"/>
+      <c r="L49" s="80"/>
+      <c r="M49" s="80"/>
+      <c r="N49" s="80"/>
       <c r="O49" s="24"/>
-      <c r="P49" s="68"/>
-      <c r="Q49" s="69"/>
-      <c r="R49" s="61"/>
-      <c r="S49" s="29"/>
-      <c r="T49" s="68"/>
+      <c r="P49" s="32"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="48"/>
+      <c r="S49" s="75"/>
+      <c r="T49" s="32"/>
       <c r="U49" s="25"/>
-      <c r="V49" s="68"/>
-      <c r="W49" s="68"/>
-      <c r="X49" s="29"/>
-      <c r="Y49" s="31"/>
+      <c r="V49" s="32"/>
+      <c r="W49" s="32"/>
+      <c r="X49" s="75"/>
+      <c r="Y49" s="77"/>
       <c r="Z49" s="12"/>
     </row>
     <row r="50" spans="4:26" ht="17.25" thickBot="1">
-      <c r="D50" s="36"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="81"/>
-      <c r="G50" s="81"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="38" t="s">
+      <c r="D50" s="67"/>
+      <c r="E50" s="73"/>
+      <c r="F50" s="73"/>
+      <c r="G50" s="73"/>
+      <c r="H50" s="73"/>
+      <c r="I50" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="J50" s="39"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="34"/>
-      <c r="M50" s="34"/>
-      <c r="N50" s="34"/>
+      <c r="J50" s="70"/>
+      <c r="K50" s="80"/>
+      <c r="L50" s="80"/>
+      <c r="M50" s="80"/>
+      <c r="N50" s="80"/>
       <c r="O50" s="24"/>
       <c r="P50" s="24"/>
-      <c r="Q50" s="64"/>
-      <c r="R50" s="61"/>
-      <c r="S50" s="29"/>
-      <c r="T50" s="67"/>
-      <c r="U50" s="68"/>
+      <c r="Q50" s="28"/>
+      <c r="R50" s="48"/>
+      <c r="S50" s="75"/>
+      <c r="T50" s="31"/>
+      <c r="U50" s="32"/>
       <c r="V50" s="25"/>
       <c r="W50" s="26"/>
-      <c r="X50" s="29"/>
-      <c r="Y50" s="31"/>
+      <c r="X50" s="75"/>
+      <c r="Y50" s="77"/>
       <c r="Z50" s="12"/>
     </row>
     <row r="51" spans="4:26">
@@ -2207,8 +2207,8 @@
       <c r="E51" s="27"/>
       <c r="F51" s="27"/>
       <c r="H51" s="27"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
+      <c r="I51" s="78"/>
+      <c r="J51" s="78"/>
       <c r="K51" s="27"/>
       <c r="L51" s="27"/>
       <c r="M51" s="27"/>
@@ -2234,11 +2234,31 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="AA29:AB29"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="E34:H38"/>
-    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K24:N50"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="E44:H50"/>
+    <mergeCell ref="S24:S50"/>
+    <mergeCell ref="X24:X50"/>
+    <mergeCell ref="D20:Y21"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="E24:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="F22:H23"/>
+    <mergeCell ref="I22:J23"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="O22:S22"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="Y24:Y50"/>
     <mergeCell ref="D34:D37"/>
     <mergeCell ref="T22:W22"/>
     <mergeCell ref="I30:J30"/>
@@ -2253,33 +2273,13 @@
     <mergeCell ref="I49:J49"/>
     <mergeCell ref="I48:J48"/>
     <mergeCell ref="I32:J32"/>
-    <mergeCell ref="D20:Y21"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="E24:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="F22:H23"/>
-    <mergeCell ref="I22:J23"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="O22:S22"/>
-    <mergeCell ref="I31:J31"/>
     <mergeCell ref="D44:D50"/>
     <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="E44:H50"/>
-    <mergeCell ref="S24:S50"/>
-    <mergeCell ref="X24:X50"/>
-    <mergeCell ref="Y24:Y50"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="K24:N50"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="AA29:AB29"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="E34:H38"/>
+    <mergeCell ref="I38:J38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>